<commit_message>
fixed links for score tables
</commit_message>
<xml_diff>
--- a/scores/exhibitions.xlsx
+++ b/scores/exhibitions.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jakob\Downloads\Dokumente\Tennis_ATP\scores\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBECF9B0-7151-4CAB-A360-A3E4C925FA8A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A942D807-C5B9-415F-8401-0480A908651A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14380" windowHeight="3980" xr2:uid="{2F90F073-1ADA-485E-A980-E00F695143FC}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14380" windowHeight="3980" activeTab="1" xr2:uid="{2F90F073-1ADA-485E-A980-E00F695143FC}"/>
   </bookViews>
   <sheets>
     <sheet name="matches" sheetId="1" r:id="rId1"/>
@@ -3450,33 +3450,6 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="21">
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
     <dxf>
       <font>
         <strike val="0"/>
@@ -3627,6 +3600,20 @@
         <shadow val="0"/>
         <u val="none"/>
         <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
         <sz val="11"/>
         <color theme="1"/>
         <name val="Arial"/>
@@ -3671,6 +3658,19 @@
         <family val="2"/>
         <scheme val="none"/>
       </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
       <font>
@@ -3781,12 +3781,12 @@
     <tableColumn id="4" xr3:uid="{EF70884D-5BEE-48D1-9C70-FB4E4652AB9E}" name="w_check" dataDxfId="15">
       <calculatedColumnFormula>IF(COUNTIF([1]!Table1[[#All],[name]],Table1[[#This Row],[winner_name]])=1,"OK","ERROR")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{56247FFB-43C6-4C13-BBA4-D109F8CF42E4}" name="l_check" dataDxfId="0">
+    <tableColumn id="5" xr3:uid="{56247FFB-43C6-4C13-BBA4-D109F8CF42E4}" name="l_check" dataDxfId="14">
       <calculatedColumnFormula>IF(COUNTIF([1]!Table1[[#All],[name]],Table1[[#This Row],[loser_name]])=1,"OK","ERROR")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{04FC4420-D69B-4651-BF63-DFB0BC97043C}" name="score" dataDxfId="14"/>
-    <tableColumn id="8" xr3:uid="{54D86A49-A18B-46DA-BD5C-1C3904958775}" name="date" dataDxfId="13"/>
-    <tableColumn id="7" xr3:uid="{F77A6AB1-0027-46E2-8E79-8B9932D98C7F}" name="city" dataDxfId="12">
+    <tableColumn id="6" xr3:uid="{04FC4420-D69B-4651-BF63-DFB0BC97043C}" name="score" dataDxfId="13"/>
+    <tableColumn id="8" xr3:uid="{54D86A49-A18B-46DA-BD5C-1C3904958775}" name="date" dataDxfId="12"/>
+    <tableColumn id="7" xr3:uid="{F77A6AB1-0027-46E2-8E79-8B9932D98C7F}" name="city" dataDxfId="11">
       <calculatedColumnFormula>VLOOKUP(Table1[[#This Row],[tourney_id]],tournaments!B:G,4,FALSE)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -3795,23 +3795,23 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{58A47B93-454B-4E2E-8821-219DBDC1DA0A}" name="Table2" displayName="Table2" ref="A1:I118" totalsRowShown="0" headerRowDxfId="11" dataDxfId="1">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{58A47B93-454B-4E2E-8821-219DBDC1DA0A}" name="Table2" displayName="Table2" ref="A1:I118" totalsRowShown="0" headerRowDxfId="10" dataDxfId="9">
   <autoFilter ref="A1:I118" xr:uid="{EC35BCDA-EA51-4179-8949-D97E950CA8D5}"/>
   <sortState ref="A2:I118">
     <sortCondition ref="B1:B118"/>
   </sortState>
   <tableColumns count="9">
-    <tableColumn id="3" xr3:uid="{D5264213-E187-4760-BAB3-56EE9B3C1F41}" name="id" dataDxfId="10">
+    <tableColumn id="3" xr3:uid="{D5264213-E187-4760-BAB3-56EE9B3C1F41}" name="id" dataDxfId="8">
       <calculatedColumnFormula>IF(Table2[[#This Row],[date]]="",Table2[[#This Row],[year]]&amp;"-"&amp;LOWER(Table2[[#This Row],[name]]),Table2[[#This Row],[year]]&amp;"-"&amp;LOWER(Table2[[#This Row],[name]])&amp;"-"&amp;YEAR(Table2[[#This Row],[date]])&amp;TEXT(Table2[[#This Row],[date]],"mm")&amp;TEXT(Table2[[#This Row],[date]],"dd"))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{4F134362-9158-4A37-9C7B-04B921BB50A4}" name="name" dataDxfId="9"/>
-    <tableColumn id="4" xr3:uid="{5E2CA73B-809D-4CBA-91B9-6A8F874F03C4}" name="year" dataDxfId="8"/>
-    <tableColumn id="1" xr3:uid="{BEEF5686-CF47-4919-9C43-13F85CC8B0E4}" name="date" dataDxfId="7"/>
-    <tableColumn id="9" xr3:uid="{A1119DBF-1628-41D5-AD41-6A5900744F3A}" name="level" dataDxfId="6"/>
-    <tableColumn id="5" xr3:uid="{FFEC4872-EE99-4B1E-850B-894CD1439D17}" name="surface" dataDxfId="5"/>
-    <tableColumn id="6" xr3:uid="{B5C01AA7-15FD-4583-BC49-DD9DEFFCF4E5}" name="outdoor" dataDxfId="4"/>
-    <tableColumn id="7" xr3:uid="{D7ED0298-B0CA-4ACB-9336-CCA9153AFD00}" name="city" dataDxfId="3"/>
-    <tableColumn id="8" xr3:uid="{94010264-C0F4-46B4-89D0-A331D4EDA41B}" name="venue" dataDxfId="2"/>
+    <tableColumn id="2" xr3:uid="{4F134362-9158-4A37-9C7B-04B921BB50A4}" name="name" dataDxfId="7"/>
+    <tableColumn id="4" xr3:uid="{5E2CA73B-809D-4CBA-91B9-6A8F874F03C4}" name="year" dataDxfId="6"/>
+    <tableColumn id="1" xr3:uid="{BEEF5686-CF47-4919-9C43-13F85CC8B0E4}" name="date" dataDxfId="5"/>
+    <tableColumn id="9" xr3:uid="{A1119DBF-1628-41D5-AD41-6A5900744F3A}" name="level" dataDxfId="4"/>
+    <tableColumn id="5" xr3:uid="{FFEC4872-EE99-4B1E-850B-894CD1439D17}" name="surface" dataDxfId="3"/>
+    <tableColumn id="6" xr3:uid="{B5C01AA7-15FD-4583-BC49-DD9DEFFCF4E5}" name="outdoor" dataDxfId="2"/>
+    <tableColumn id="7" xr3:uid="{D7ED0298-B0CA-4ACB-9336-CCA9153AFD00}" name="city" dataDxfId="1"/>
+    <tableColumn id="8" xr3:uid="{94010264-C0F4-46B4-89D0-A331D4EDA41B}" name="venue" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -4116,7 +4116,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B62B63A7-71FC-42FD-A4A5-456CFA98E8BF}">
   <dimension ref="A1:I1321"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -42453,8 +42453,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B50D9011-4C8E-4BB4-BF80-0AA0793D869B}">
   <dimension ref="A1:J118"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -42468,8 +42468,7 @@
     <col min="7" max="7" width="10.36328125" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="39" style="1" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="34.26953125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="33.1796875" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="16384" width="8.7265625" style="1"/>
+    <col min="11" max="16384" width="8.7265625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="14" x14ac:dyDescent="0.3">

</xml_diff>